<commit_message>
Core Java Day 1
</commit_message>
<xml_diff>
--- a/Training Schedule.xlsx
+++ b/Training Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vivek Gohil\Training\Mindgate-Chennai-July-2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C6CD2F4-1F3F-49BF-BBF1-C3A3F97B30E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D527F7B7-3404-4432-801D-D5402FFC4BD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17500" xr2:uid="{90E3184F-508F-4A14-AAD6-801FB3A1F894}"/>
+    <workbookView xWindow="0" yWindow="15" windowWidth="19200" windowHeight="10065" xr2:uid="{90E3184F-508F-4A14-AAD6-801FB3A1F894}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Sr Number</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>Project</t>
+  </si>
+  <si>
+    <t>Review</t>
   </si>
 </sst>
 </file>
@@ -145,12 +148,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,200 +469,271 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFE9025E-7070-4856-8DF7-2297080970DE}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.54296875" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
+      <c r="C3" s="2">
+        <v>45852</v>
+      </c>
+      <c r="D3" s="2">
+        <v>45853</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
+      <c r="C4" s="2">
+        <v>45845</v>
+      </c>
+      <c r="D4" s="2">
+        <v>45854</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
+      <c r="C5" s="2">
+        <v>45855</v>
+      </c>
+      <c r="D5" s="2">
+        <v>45856</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
+      <c r="C6" s="2">
+        <v>45859</v>
+      </c>
+      <c r="D6" s="2">
+        <v>45859</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
+      <c r="C7" s="2">
+        <v>45860</v>
+      </c>
+      <c r="D7" s="2">
+        <v>45861</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="2">
+      <c r="C8" s="2">
+        <v>45862</v>
+      </c>
+      <c r="D8" s="2">
+        <v>45862</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="2">
+      <c r="C9" s="2">
+        <v>45863</v>
+      </c>
+      <c r="D9" s="2">
+        <v>45863</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="2">
+      <c r="C10" s="2">
+        <v>45866</v>
+      </c>
+      <c r="D10" s="2">
+        <v>45867</v>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="2">
+      <c r="C11" s="2">
+        <v>45868</v>
+      </c>
+      <c r="D11" s="2">
+        <v>45869</v>
+      </c>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="2">
+      <c r="C12" s="2">
+        <v>45870</v>
+      </c>
+      <c r="D12" s="2">
+        <v>45870</v>
+      </c>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="2">
+      <c r="C13" s="2">
+        <v>45873</v>
+      </c>
+      <c r="D13" s="2">
+        <v>45874</v>
+      </c>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="2">
+      <c r="C14" s="2">
+        <v>45875</v>
+      </c>
+      <c r="D14" s="2">
+        <v>45875</v>
+      </c>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="2">
+      <c r="C15" s="2">
+        <v>45876</v>
+      </c>
+      <c r="D15" s="2">
+        <v>45876</v>
+      </c>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="C16" s="2">
+        <v>45877</v>
+      </c>
+      <c r="D16" s="2">
+        <v>45889</v>
+      </c>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="2">
+        <v>45890</v>
+      </c>
+      <c r="D17" s="2">
+        <v>45891</v>
+      </c>
+      <c r="E17" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -674,7 +749,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>